<commit_message>
commit Linked List feature file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LoginTestData.xlsx
+++ b/src/test/resources/TestData/LoginTestData.xlsx
@@ -3,20 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{894A0901-1EF0-4757-9165-7A04285F3BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\god\eclipse-workspace\DS-AlgoProj\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271C1BFC-C282-4FB2-A43B-62BFEA0AD656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="251" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="PythonCode" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Vijayabharathi</t>
   </si>
@@ -43,13 +48,101 @@
   </si>
   <si>
     <t>TC001</t>
+  </si>
+  <si>
+    <t>pythonCode</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>print("hello");</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>def search(input_list, num):
+if(num in input_list):
+print("Element Found")
+\b
+\b
+else:
+print("Not Found")
+\b
+\b
+\b
+\b
+search([12, 23, 45, 67, 6, 90] , 12)</t>
+  </si>
+  <si>
+    <t>Element Found</t>
+  </si>
+  <si>
+    <t>submission success</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums) :
+count = 0
+result = 0
+for i in range(0, len(nums)):
+if (nums[i] == 0):
+count = 0
+\b
+\b
+else:
+count+= 1
+\b
+\b
+result = max(result, count)
+\b
+\b
+print(result)
+\b
+\b
+findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+c=0
+for i in nums:
+j=str(i)
+x=len(j)
+if x%2==0:
+c=c+1
+\b
+\b
+\b
+\b
+print c
+return c
+findNumbers([12,345,2,6,7896])</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+squares_list = []
+for i in range(0, len(nums)):
+square = nums[i] * nums[i];
+squares_list.append(square)
+\b
+\b
+sorted_squares_list = sorted(squares_list)
+print sorted_squares_list;
+return sorted_squares_list;
+sortedSquares([-7,-3,2,3,11])</t>
+  </si>
+  <si>
+    <t>[4, 9, 9, 49, 121]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -69,13 +162,30 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -87,17 +197,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{9CF959E7-BF56-4114-B72F-51C413945FB0}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -411,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -451,17 +568,116 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="O13" t="s">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08157208-34A5-4823-827D-AB44E091375F}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="243.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commiting updated test Data sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LoginTestData.xlsx
+++ b/src/test/resources/TestData/LoginTestData.xlsx
@@ -3,25 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\god\eclipse-workspace\DS-AlgoProj\src\test\resources\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271C1BFC-C282-4FB2-A43B-62BFEA0AD656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5618DA00-8B36-4B95-BB58-40D2798BBD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="251" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="251" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginSheet" sheetId="1" r:id="rId1"/>
-    <sheet name="PythonCode" sheetId="2" r:id="rId2"/>
+    <sheet name="pythonCode" sheetId="2" r:id="rId2"/>
+    <sheet name="Practice Qns" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>Vijayabharathi</t>
   </si>
@@ -54,9 +51,6 @@
   </si>
   <si>
     <t>Result</t>
-  </si>
-  <si>
-    <t>print("hello");</t>
   </si>
   <si>
     <t>hello</t>
@@ -136,6 +130,21 @@
   </si>
   <si>
     <t>[4, 9, 9, 49, 121]</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>print("hello")</t>
+  </si>
+  <si>
+    <t>print("Hello")</t>
+  </si>
+  <si>
+    <t>TestId</t>
   </si>
 </sst>
 </file>
@@ -206,11 +215,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,9 +537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -580,104 +587,182 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08157208-34A5-4823-827D-AB44E091375F}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="243.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="243.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB2F416-0080-4CD5-8640-78BD573AE583}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="243.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="6" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="6" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test data excel commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LoginTestData.xlsx
+++ b/src/test/resources/TestData/LoginTestData.xlsx
@@ -3,25 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\god\eclipse-workspace\DS-AlgoProj\src\test\resources\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271C1BFC-C282-4FB2-A43B-62BFEA0AD656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5618DA00-8B36-4B95-BB58-40D2798BBD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="251" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="251" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginSheet" sheetId="1" r:id="rId1"/>
-    <sheet name="PythonCode" sheetId="2" r:id="rId2"/>
+    <sheet name="pythonCode" sheetId="2" r:id="rId2"/>
+    <sheet name="Practice Qns" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>Vijayabharathi</t>
   </si>
@@ -54,9 +51,6 @@
   </si>
   <si>
     <t>Result</t>
-  </si>
-  <si>
-    <t>print("hello");</t>
   </si>
   <si>
     <t>hello</t>
@@ -136,6 +130,21 @@
   </si>
   <si>
     <t>[4, 9, 9, 49, 121]</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>print("hello")</t>
+  </si>
+  <si>
+    <t>print("Hello")</t>
+  </si>
+  <si>
+    <t>TestId</t>
   </si>
 </sst>
 </file>
@@ -206,11 +215,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,9 +537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -580,104 +587,182 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08157208-34A5-4823-827D-AB44E091375F}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="243.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="243.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB2F416-0080-4CD5-8640-78BD573AE583}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="243.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="6" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="6" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>